<commit_message>
Update: Removed stochastic and simplified MACD logic
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>43.54</v>
+        <v>60.8</v>
       </c>
       <c r="C2" s="7" t="n"/>
       <c r="D2" s="8" t="n"/>
@@ -518,19 +518,19 @@
         </is>
       </c>
       <c r="B3" s="6" t="n">
-        <v>35.14</v>
-      </c>
-      <c r="C3" s="7" t="n"/>
+        <v>37.36</v>
+      </c>
+      <c r="C3" s="9" t="n"/>
       <c r="D3" s="9" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>XLY</t>
+          <t>XLF</t>
         </is>
       </c>
       <c r="B4" s="6" t="n">
-        <v>15.87</v>
+        <v>17.74</v>
       </c>
       <c r="C4" s="9" t="n"/>
       <c r="D4" s="8" t="n"/>
@@ -538,11 +538,11 @@
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>XLF</t>
+          <t>XLY</t>
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>14.98</v>
+        <v>16.68</v>
       </c>
       <c r="C5" s="9" t="n"/>
       <c r="D5" s="8" t="n"/>
@@ -550,47 +550,47 @@
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>GLD</t>
+          <t>MTUM</t>
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>13.83</v>
+        <v>15.87</v>
       </c>
       <c r="C6" s="9" t="n"/>
-      <c r="D6" s="9" t="n"/>
+      <c r="D6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>MTUM</t>
+          <t>GLD</t>
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>11.3</v>
+        <v>15.66</v>
       </c>
       <c r="C7" s="9" t="n"/>
-      <c r="D7" s="8" t="n"/>
+      <c r="D7" s="9" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>SPYG</t>
+          <t>SLV</t>
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>8.85</v>
+        <v>12.83</v>
       </c>
       <c r="C8" s="9" t="n"/>
-      <c r="D8" s="8" t="n"/>
+      <c r="D8" s="9" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>UUP</t>
+          <t>SPYG</t>
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>8.65</v>
+        <v>12.18</v>
       </c>
       <c r="C9" s="9" t="n"/>
       <c r="D9" s="8" t="n"/>
@@ -598,23 +598,23 @@
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>SLV</t>
+          <t>QQQ</t>
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>7.44</v>
-      </c>
-      <c r="C10" s="7" t="n"/>
-      <c r="D10" s="9" t="n"/>
+        <v>11.11</v>
+      </c>
+      <c r="C10" s="9" t="n"/>
+      <c r="D10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>QQQ</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="B11" s="6" t="n">
-        <v>7.02</v>
+        <v>8.73</v>
       </c>
       <c r="C11" s="9" t="n"/>
       <c r="D11" s="8" t="n"/>
@@ -622,11 +622,11 @@
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>SPY</t>
+          <t>UUP</t>
         </is>
       </c>
       <c r="B12" s="6" t="n">
-        <v>6.09</v>
+        <v>7.96</v>
       </c>
       <c r="C12" s="9" t="n"/>
       <c r="D12" s="8" t="n"/>
@@ -634,11 +634,11 @@
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>XLU</t>
+          <t>XLI</t>
         </is>
       </c>
       <c r="B13" s="6" t="n">
-        <v>5.41</v>
+        <v>7.64</v>
       </c>
       <c r="C13" s="9" t="n"/>
       <c r="D13" s="8" t="n"/>
@@ -646,47 +646,47 @@
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>XLI</t>
+          <t>XLK</t>
         </is>
       </c>
       <c r="B14" s="6" t="n">
-        <v>4.56</v>
-      </c>
-      <c r="C14" s="9" t="n"/>
+        <v>7.6</v>
+      </c>
+      <c r="C14" s="7" t="n"/>
       <c r="D14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>RSP</t>
+          <t>USO</t>
         </is>
       </c>
       <c r="B15" s="6" t="n">
-        <v>3.22</v>
-      </c>
-      <c r="C15" s="9" t="n"/>
+        <v>6.37</v>
+      </c>
+      <c r="C15" s="8" t="n"/>
       <c r="D15" s="8" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>GMF</t>
+          <t>XLU</t>
         </is>
       </c>
       <c r="B16" s="6" t="n">
-        <v>3.01</v>
-      </c>
-      <c r="C16" s="7" t="n"/>
+        <v>6.09</v>
+      </c>
+      <c r="C16" s="9" t="n"/>
       <c r="D16" s="8" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>XLK</t>
+          <t>RSP</t>
         </is>
       </c>
       <c r="B17" s="6" t="n">
-        <v>2.71</v>
+        <v>5.36</v>
       </c>
       <c r="C17" s="9" t="n"/>
       <c r="D17" s="8" t="n"/>
@@ -694,47 +694,47 @@
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>XLP</t>
+          <t>GMF</t>
         </is>
       </c>
       <c r="B18" s="6" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="C18" s="9" t="n"/>
-      <c r="D18" s="9" t="n"/>
+        <v>5.12</v>
+      </c>
+      <c r="C18" s="7" t="n"/>
+      <c r="D18" s="8" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>SPYV</t>
+          <t>XLE</t>
         </is>
       </c>
       <c r="B19" s="6" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="C19" s="9" t="n"/>
+        <v>3.81</v>
+      </c>
+      <c r="C19" s="7" t="n"/>
       <c r="D19" s="8" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>XLE</t>
+          <t>SPYV</t>
         </is>
       </c>
       <c r="B20" s="6" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="C20" s="7" t="n"/>
-      <c r="D20" s="9" t="n"/>
+        <v>3.4</v>
+      </c>
+      <c r="C20" s="9" t="n"/>
+      <c r="D20" s="8" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>USO</t>
+          <t>IWO</t>
         </is>
       </c>
       <c r="B21" s="6" t="n">
-        <v>1.18</v>
+        <v>2.01</v>
       </c>
       <c r="C21" s="7" t="n"/>
       <c r="D21" s="8" t="n"/>
@@ -742,38 +742,38 @@
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>XLRE</t>
+          <t>XLP</t>
         </is>
       </c>
       <c r="B22" s="6" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="C22" s="7" t="n"/>
-      <c r="D22" s="8" t="n"/>
+        <v>1.94</v>
+      </c>
+      <c r="C22" s="9" t="n"/>
+      <c r="D22" s="9" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>IWO</t>
-        </is>
-      </c>
-      <c r="B23" s="10" t="n">
-        <v>-0.9</v>
-      </c>
-      <c r="C23" s="7" t="n"/>
-      <c r="D23" s="8" t="n"/>
+          <t>XLRE</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="C23" s="9" t="n"/>
+      <c r="D23" s="9" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="inlineStr">
         <is>
-          <t>TLT</t>
-        </is>
-      </c>
-      <c r="B24" s="10" t="n">
-        <v>-2.2</v>
-      </c>
-      <c r="C24" s="7" t="n"/>
-      <c r="D24" s="9" t="n"/>
+          <t>IWN</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C24" s="8" t="n"/>
+      <c r="D24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="inlineStr">
@@ -782,46 +782,46 @@
         </is>
       </c>
       <c r="B25" s="10" t="n">
-        <v>-2.33</v>
-      </c>
-      <c r="C25" s="9" t="n"/>
+        <v>-0.88</v>
+      </c>
+      <c r="C25" s="7" t="n"/>
       <c r="D25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="inlineStr">
         <is>
-          <t>IWN</t>
+          <t>XLV</t>
         </is>
       </c>
       <c r="B26" s="10" t="n">
-        <v>-2.98</v>
+        <v>-2.03</v>
       </c>
       <c r="C26" s="7" t="n"/>
-      <c r="D26" s="8" t="n"/>
+      <c r="D26" s="9" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>XLB</t>
         </is>
       </c>
       <c r="B27" s="10" t="n">
-        <v>-4.48</v>
+        <v>-2.3</v>
       </c>
       <c r="C27" s="7" t="n"/>
-      <c r="D27" s="9" t="n"/>
+      <c r="D27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="inlineStr">
         <is>
-          <t>XLB</t>
+          <t>TLT</t>
         </is>
       </c>
       <c r="B28" s="10" t="n">
-        <v>-4.94</v>
-      </c>
-      <c r="C28" s="7" t="n"/>
-      <c r="D28" s="8" t="n"/>
+        <v>-5.07</v>
+      </c>
+      <c r="C28" s="9" t="n"/>
+      <c r="D28" s="9" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Correcciones en funciones get_macd_signal y get_trimestral_signal para manejar correctamente pandas Series
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -36,7 +36,7 @@
       <color rgb="009C0006"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -67,6 +67,18 @@
         <bgColor rgb="004472C4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0087CEEB"/>
+        <bgColor rgb="0087CEEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFA500"/>
+        <bgColor rgb="00FFA500"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -86,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -98,6 +110,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -463,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,9 +486,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="7" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -498,6 +514,16 @@
           <t>Semanal</t>
         </is>
       </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Trimestral</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Señal</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
@@ -506,70 +532,82 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>60.8</v>
+        <v>36.02</v>
       </c>
       <c r="C2" s="7" t="n"/>
       <c r="D2" s="8" t="n"/>
+      <c r="E2" s="9" t="n"/>
+      <c r="F2" s="5" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>FXI</t>
+          <t>GLD</t>
         </is>
       </c>
       <c r="B3" s="6" t="n">
-        <v>37.36</v>
+        <v>23.45</v>
       </c>
       <c r="C3" s="9" t="n"/>
       <c r="D3" s="9" t="n"/>
+      <c r="E3" s="9" t="n"/>
+      <c r="F3" s="5" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>XLF</t>
+          <t>FXI</t>
         </is>
       </c>
       <c r="B4" s="6" t="n">
-        <v>17.74</v>
-      </c>
-      <c r="C4" s="9" t="n"/>
+        <v>7.88</v>
+      </c>
+      <c r="C4" s="7" t="n"/>
       <c r="D4" s="8" t="n"/>
+      <c r="E4" s="8" t="n"/>
+      <c r="F4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>XLY</t>
+          <t>XLP</t>
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>16.68</v>
+        <v>2.87</v>
       </c>
       <c r="C5" s="9" t="n"/>
-      <c r="D5" s="8" t="n"/>
+      <c r="D5" s="9" t="n"/>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="12" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>MTUM</t>
+          <t>XLF</t>
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>15.87</v>
+        <v>1.77</v>
       </c>
       <c r="C6" s="9" t="n"/>
       <c r="D6" s="8" t="n"/>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="11" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>GLD</t>
-        </is>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>15.66</v>
+          <t>XLU</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>-1.6</v>
       </c>
       <c r="C7" s="9" t="n"/>
-      <c r="D7" s="9" t="n"/>
+      <c r="D7" s="8" t="n"/>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="11" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
@@ -577,143 +615,167 @@
           <t>SLV</t>
         </is>
       </c>
-      <c r="B8" s="6" t="n">
-        <v>12.83</v>
+      <c r="B8" s="10" t="n">
+        <v>-2.2</v>
       </c>
       <c r="C8" s="9" t="n"/>
-      <c r="D8" s="9" t="n"/>
+      <c r="D8" s="8" t="n"/>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>SPYG</t>
-        </is>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>12.18</v>
-      </c>
-      <c r="C9" s="9" t="n"/>
+          <t>UUP</t>
+        </is>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>-3.13</v>
+      </c>
+      <c r="C9" s="8" t="n"/>
       <c r="D9" s="8" t="n"/>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="5" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>QQQ</t>
-        </is>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>11.11</v>
-      </c>
-      <c r="C10" s="9" t="n"/>
+          <t>TLT</t>
+        </is>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>-3.64</v>
+      </c>
+      <c r="C10" s="7" t="n"/>
       <c r="D10" s="8" t="n"/>
+      <c r="E10" s="8" t="n"/>
+      <c r="F10" s="11" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>SPY</t>
-        </is>
-      </c>
-      <c r="B11" s="6" t="n">
-        <v>8.73</v>
-      </c>
-      <c r="C11" s="9" t="n"/>
+          <t>MTUM</t>
+        </is>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>-4.06</v>
+      </c>
+      <c r="C11" s="7" t="n"/>
       <c r="D11" s="8" t="n"/>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="5" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>UUP</t>
-        </is>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>7.96</v>
-      </c>
-      <c r="C12" s="9" t="n"/>
+          <t>USO</t>
+        </is>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>-5.4</v>
+      </c>
+      <c r="C12" s="8" t="n"/>
       <c r="D12" s="8" t="n"/>
+      <c r="E12" s="8" t="n"/>
+      <c r="F12" s="5" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>XLI</t>
-        </is>
-      </c>
-      <c r="B13" s="6" t="n">
-        <v>7.64</v>
-      </c>
-      <c r="C13" s="9" t="n"/>
+          <t>XLY</t>
+        </is>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>-6.05</v>
+      </c>
+      <c r="C13" s="7" t="n"/>
       <c r="D13" s="8" t="n"/>
+      <c r="E13" s="9" t="n"/>
+      <c r="F13" s="5" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>XLK</t>
-        </is>
-      </c>
-      <c r="B14" s="6" t="n">
-        <v>7.6</v>
+          <t>XLRE</t>
+        </is>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>-6.5</v>
       </c>
       <c r="C14" s="7" t="n"/>
       <c r="D14" s="8" t="n"/>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="5" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>USO</t>
-        </is>
-      </c>
-      <c r="B15" s="6" t="n">
-        <v>6.37</v>
+          <t>XLI</t>
+        </is>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>-6.85</v>
       </c>
       <c r="C15" s="8" t="n"/>
       <c r="D15" s="8" t="n"/>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="5" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>XLU</t>
-        </is>
-      </c>
-      <c r="B16" s="6" t="n">
-        <v>6.09</v>
-      </c>
-      <c r="C16" s="9" t="n"/>
+          <t>GMF</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="n">
+        <v>-7.11</v>
+      </c>
+      <c r="C16" s="7" t="n"/>
       <c r="D16" s="8" t="n"/>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="11" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>RSP</t>
-        </is>
-      </c>
-      <c r="B17" s="6" t="n">
-        <v>5.36</v>
-      </c>
-      <c r="C17" s="9" t="n"/>
+          <t>XLE</t>
+        </is>
+      </c>
+      <c r="B17" s="10" t="n">
+        <v>-7.21</v>
+      </c>
+      <c r="C17" s="8" t="n"/>
       <c r="D17" s="8" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="11" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>GMF</t>
-        </is>
-      </c>
-      <c r="B18" s="6" t="n">
-        <v>5.12</v>
-      </c>
-      <c r="C18" s="7" t="n"/>
+          <t>RSP</t>
+        </is>
+      </c>
+      <c r="B18" s="10" t="n">
+        <v>-7.36</v>
+      </c>
+      <c r="C18" s="8" t="n"/>
       <c r="D18" s="8" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="5" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>XLE</t>
-        </is>
-      </c>
-      <c r="B19" s="6" t="n">
-        <v>3.81</v>
-      </c>
-      <c r="C19" s="7" t="n"/>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="B19" s="10" t="n">
+        <v>-8.07</v>
+      </c>
+      <c r="C19" s="8" t="n"/>
       <c r="D19" s="8" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="5" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
@@ -721,59 +783,69 @@
           <t>SPYV</t>
         </is>
       </c>
-      <c r="B20" s="6" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="C20" s="9" t="n"/>
+      <c r="B20" s="10" t="n">
+        <v>-8.23</v>
+      </c>
+      <c r="C20" s="8" t="n"/>
       <c r="D20" s="8" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="5" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>IWO</t>
-        </is>
-      </c>
-      <c r="B21" s="6" t="n">
-        <v>2.01</v>
-      </c>
-      <c r="C21" s="7" t="n"/>
+          <t>XLV</t>
+        </is>
+      </c>
+      <c r="B21" s="10" t="n">
+        <v>-8.43</v>
+      </c>
+      <c r="C21" s="8" t="n"/>
       <c r="D21" s="8" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="11" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>XLP</t>
-        </is>
-      </c>
-      <c r="B22" s="6" t="n">
-        <v>1.94</v>
-      </c>
-      <c r="C22" s="9" t="n"/>
-      <c r="D22" s="9" t="n"/>
+          <t>SPYG</t>
+        </is>
+      </c>
+      <c r="B22" s="10" t="n">
+        <v>-8.77</v>
+      </c>
+      <c r="C22" s="8" t="n"/>
+      <c r="D22" s="8" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="5" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>XLRE</t>
-        </is>
-      </c>
-      <c r="B23" s="6" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="C23" s="9" t="n"/>
-      <c r="D23" s="9" t="n"/>
+          <t>QQQ</t>
+        </is>
+      </c>
+      <c r="B23" s="10" t="n">
+        <v>-9.43</v>
+      </c>
+      <c r="C23" s="8" t="n"/>
+      <c r="D23" s="8" t="n"/>
+      <c r="E23" s="9" t="n"/>
+      <c r="F23" s="5" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="inlineStr">
         <is>
-          <t>IWN</t>
-        </is>
-      </c>
-      <c r="B24" s="6" t="n">
-        <v>0.02</v>
+          <t>XLB</t>
+        </is>
+      </c>
+      <c r="B24" s="10" t="n">
+        <v>-12.35</v>
       </c>
       <c r="C24" s="8" t="n"/>
       <c r="D24" s="8" t="n"/>
+      <c r="E24" s="9" t="n"/>
+      <c r="F24" s="5" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="inlineStr">
@@ -782,46 +854,54 @@
         </is>
       </c>
       <c r="B25" s="10" t="n">
-        <v>-0.88</v>
-      </c>
-      <c r="C25" s="7" t="n"/>
+        <v>-12.8</v>
+      </c>
+      <c r="C25" s="8" t="n"/>
       <c r="D25" s="8" t="n"/>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="5" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>IWN</t>
         </is>
       </c>
       <c r="B26" s="10" t="n">
-        <v>-2.03</v>
-      </c>
-      <c r="C26" s="7" t="n"/>
-      <c r="D26" s="9" t="n"/>
+        <v>-13.37</v>
+      </c>
+      <c r="C26" s="8" t="n"/>
+      <c r="D26" s="8" t="n"/>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="5" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
-          <t>XLB</t>
+          <t>IWO</t>
         </is>
       </c>
       <c r="B27" s="10" t="n">
-        <v>-2.3</v>
-      </c>
-      <c r="C27" s="7" t="n"/>
+        <v>-14.09</v>
+      </c>
+      <c r="C27" s="8" t="n"/>
       <c r="D27" s="8" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="5" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="inlineStr">
         <is>
-          <t>TLT</t>
+          <t>XLK</t>
         </is>
       </c>
       <c r="B28" s="10" t="n">
-        <v>-5.07</v>
-      </c>
-      <c r="C28" s="9" t="n"/>
-      <c r="D28" s="9" t="n"/>
+        <v>-15.77</v>
+      </c>
+      <c r="C28" s="8" t="n"/>
+      <c r="D28" s="8" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="5" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add GitHub Actions workflow for building executable
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>36.02</v>
+        <v>37.02</v>
       </c>
       <c r="C2" s="7" t="n"/>
       <c r="D2" s="8" t="n"/>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B3" s="6" t="n">
-        <v>23.45</v>
+        <v>22.81</v>
       </c>
       <c r="C3" s="9" t="n"/>
       <c r="D3" s="9" t="n"/>
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B4" s="6" t="n">
-        <v>7.88</v>
+        <v>7.06</v>
       </c>
       <c r="C4" s="7" t="n"/>
       <c r="D4" s="8" t="n"/>
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>2.87</v>
+        <v>2.77</v>
       </c>
       <c r="C5" s="9" t="n"/>
       <c r="D5" s="9" t="n"/>
@@ -588,7 +588,7 @@
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>1.77</v>
+        <v>1.94</v>
       </c>
       <c r="C6" s="9" t="n"/>
       <c r="D6" s="8" t="n"/>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B7" s="10" t="n">
-        <v>-1.6</v>
+        <v>-1.46</v>
       </c>
       <c r="C7" s="9" t="n"/>
       <c r="D7" s="8" t="n"/>
@@ -612,13 +612,13 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>SLV</t>
+          <t>UUP</t>
         </is>
       </c>
       <c r="B8" s="10" t="n">
-        <v>-2.2</v>
-      </c>
-      <c r="C8" s="9" t="n"/>
+        <v>-2.95</v>
+      </c>
+      <c r="C8" s="8" t="n"/>
       <c r="D8" s="8" t="n"/>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="5" t="n"/>
@@ -626,13 +626,13 @@
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>UUP</t>
+          <t>SLV</t>
         </is>
       </c>
       <c r="B9" s="10" t="n">
-        <v>-3.13</v>
-      </c>
-      <c r="C9" s="8" t="n"/>
+        <v>-3.69</v>
+      </c>
+      <c r="C9" s="9" t="n"/>
       <c r="D9" s="8" t="n"/>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="5" t="n"/>
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="B10" s="10" t="n">
-        <v>-3.64</v>
+        <v>-4.15</v>
       </c>
       <c r="C10" s="7" t="n"/>
       <c r="D10" s="8" t="n"/>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="B11" s="10" t="n">
-        <v>-4.06</v>
+        <v>-4.52</v>
       </c>
       <c r="C11" s="7" t="n"/>
       <c r="D11" s="8" t="n"/>
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B12" s="10" t="n">
-        <v>-5.4</v>
+        <v>-6.55</v>
       </c>
       <c r="C12" s="8" t="n"/>
       <c r="D12" s="8" t="n"/>
@@ -682,11 +682,11 @@
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>XLY</t>
+          <t>XLRE</t>
         </is>
       </c>
       <c r="B13" s="10" t="n">
-        <v>-6.05</v>
+        <v>-6.7</v>
       </c>
       <c r="C13" s="7" t="n"/>
       <c r="D13" s="8" t="n"/>
@@ -696,13 +696,13 @@
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>XLRE</t>
+          <t>XLY</t>
         </is>
       </c>
       <c r="B14" s="10" t="n">
-        <v>-6.5</v>
-      </c>
-      <c r="C14" s="7" t="n"/>
+        <v>-6.86</v>
+      </c>
+      <c r="C14" s="8" t="n"/>
       <c r="D14" s="8" t="n"/>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="5" t="n"/>
@@ -710,81 +710,81 @@
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>XLI</t>
+          <t>GMF</t>
         </is>
       </c>
       <c r="B15" s="10" t="n">
-        <v>-6.85</v>
-      </c>
-      <c r="C15" s="8" t="n"/>
+        <v>-7.17</v>
+      </c>
+      <c r="C15" s="7" t="n"/>
       <c r="D15" s="8" t="n"/>
       <c r="E15" s="9" t="n"/>
-      <c r="F15" s="5" t="n"/>
+      <c r="F15" s="11" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>GMF</t>
+          <t>XLI</t>
         </is>
       </c>
       <c r="B16" s="10" t="n">
-        <v>-7.11</v>
-      </c>
-      <c r="C16" s="7" t="n"/>
+        <v>-7.21</v>
+      </c>
+      <c r="C16" s="8" t="n"/>
       <c r="D16" s="8" t="n"/>
       <c r="E16" s="9" t="n"/>
-      <c r="F16" s="11" t="n"/>
+      <c r="F16" s="5" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>XLE</t>
+          <t>RSP</t>
         </is>
       </c>
       <c r="B17" s="10" t="n">
-        <v>-7.21</v>
+        <v>-7.54</v>
       </c>
       <c r="C17" s="8" t="n"/>
       <c r="D17" s="8" t="n"/>
       <c r="E17" s="9" t="n"/>
-      <c r="F17" s="11" t="n"/>
+      <c r="F17" s="5" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>RSP</t>
+          <t>XLE</t>
         </is>
       </c>
       <c r="B18" s="10" t="n">
-        <v>-7.36</v>
+        <v>-7.86</v>
       </c>
       <c r="C18" s="8" t="n"/>
       <c r="D18" s="8" t="n"/>
       <c r="E18" s="9" t="n"/>
-      <c r="F18" s="5" t="n"/>
+      <c r="F18" s="11" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>SPY</t>
+          <t>XLV</t>
         </is>
       </c>
       <c r="B19" s="10" t="n">
-        <v>-8.07</v>
+        <v>-8.34</v>
       </c>
       <c r="C19" s="8" t="n"/>
       <c r="D19" s="8" t="n"/>
       <c r="E19" s="9" t="n"/>
-      <c r="F19" s="5" t="n"/>
+      <c r="F19" s="11" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>SPYV</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="B20" s="10" t="n">
-        <v>-8.23</v>
+        <v>-8.359999999999999</v>
       </c>
       <c r="C20" s="8" t="n"/>
       <c r="D20" s="8" t="n"/>
@@ -794,16 +794,16 @@
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>SPYV</t>
         </is>
       </c>
       <c r="B21" s="10" t="n">
-        <v>-8.43</v>
+        <v>-8.44</v>
       </c>
       <c r="C21" s="8" t="n"/>
       <c r="D21" s="8" t="n"/>
       <c r="E21" s="9" t="n"/>
-      <c r="F21" s="11" t="n"/>
+      <c r="F21" s="5" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B22" s="10" t="n">
-        <v>-8.77</v>
+        <v>-9.210000000000001</v>
       </c>
       <c r="C22" s="8" t="n"/>
       <c r="D22" s="8" t="n"/>
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="B23" s="10" t="n">
-        <v>-9.43</v>
+        <v>-9.99</v>
       </c>
       <c r="C23" s="8" t="n"/>
       <c r="D23" s="8" t="n"/>
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="B24" s="10" t="n">
-        <v>-12.35</v>
+        <v>-12.52</v>
       </c>
       <c r="C24" s="8" t="n"/>
       <c r="D24" s="8" t="n"/>
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="B25" s="10" t="n">
-        <v>-12.8</v>
+        <v>-13.18</v>
       </c>
       <c r="C25" s="8" t="n"/>
       <c r="D25" s="8" t="n"/>
@@ -868,7 +868,7 @@
         </is>
       </c>
       <c r="B26" s="10" t="n">
-        <v>-13.37</v>
+        <v>-13.51</v>
       </c>
       <c r="C26" s="8" t="n"/>
       <c r="D26" s="8" t="n"/>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B27" s="10" t="n">
-        <v>-14.09</v>
+        <v>-14.37</v>
       </c>
       <c r="C27" s="8" t="n"/>
       <c r="D27" s="8" t="n"/>
@@ -896,7 +896,7 @@
         </is>
       </c>
       <c r="B28" s="10" t="n">
-        <v>-15.77</v>
+        <v>-16.14</v>
       </c>
       <c r="C28" s="8" t="n"/>
       <c r="D28" s="8" t="n"/>

</xml_diff>